<commit_message>
Research done, it juste to be make clean notebook
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_6\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A02CC08-CBBA-4D40-9092-89CEFD1DC0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BEFCF-95DA-4D85-9BFC-3AA732610E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -117,44 +117,69 @@
     <t>le graphique réalisé est lisible et compréhensible (ex : taille des titres et légende)</t>
   </si>
   <si>
-    <t>lowercase, retrait des mot parasite</t>
-  </si>
-  <si>
-    <t>tokenisation</t>
-  </si>
-  <si>
-    <t>Nettoyage text done</t>
-  </si>
-  <si>
-    <t>Tri à faire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A finaliser à la fin </t>
-  </si>
-  <si>
     <t>Archivé et daté</t>
   </si>
   <si>
     <t>ETL fonctionnel</t>
   </si>
   <si>
-    <t>Text ? Sur image faisable et à faire</t>
-  </si>
-  <si>
-    <t>à voir, préserver un maximum de variance de préférence</t>
-  </si>
-  <si>
-    <t>Text ne me semble à l'heure actuel peu intéressant</t>
-  </si>
-  <si>
     <t>Partie a faire avec Flask / AmChart</t>
+  </si>
+  <si>
+    <t>Tri plus approfondi possible</t>
+  </si>
+  <si>
+    <t>utilisation après coup de AmChart ou si pas de temps Voilà</t>
+  </si>
+  <si>
+    <t>lowercase, retrait des mot parasite (stop_word)</t>
+  </si>
+  <si>
+    <t>SIFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP :NMF voir pour LSA/PLSA/LDA - CV : PCA sur SIFT  </t>
+  </si>
+  <si>
+    <t>NLP : T-SNE à 2D (visualisation) CV : T-SNE également</t>
+  </si>
+  <si>
+    <t>cv2 blur</t>
+  </si>
+  <si>
+    <t>cv2 equalizeHist</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nettoyage text done NLP création de pipeline et CV en cours </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>FAIRE DES PIPELINE</t>
+    </r>
+  </si>
+  <si>
+    <t>NLP : Reduction du temps de calcul et surtout création de la matrice sujet-terme par factorisation</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>TFIDvectorizer /BOW stop_word lemma spacy ET sift + kmeans (bag of visual word)</t>
+  </si>
+  <si>
+    <t>tokenisation et lemmatization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +225,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Montserrat"/>
     </font>
   </fonts>
   <fills count="11">
@@ -801,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,7 +866,7 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C8,C10:C16,C18:C20,C22:C25)</f>
-        <v>0.29444444444444445</v>
+        <v>0.85000000000000009</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -847,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -855,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>30</v>
@@ -866,10 +896,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -880,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -898,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="64" customHeight="1" x14ac:dyDescent="0.35">
@@ -909,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
@@ -917,36 +947,44 @@
         <v>13</v>
       </c>
       <c r="C12" s="12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="12">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="2:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="12">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="2:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="13">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" t="s">
         <v>4</v>
       </c>
@@ -956,10 +994,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="14">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -974,21 +1012,21 @@
         <v>19</v>
       </c>
       <c r="C18" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="99" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -996,7 +1034,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="14">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>35</v>
@@ -1008,7 +1046,7 @@
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1016,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="15"/>
     </row>
@@ -1025,16 +1063,18 @@
         <v>24</v>
       </c>
       <c r="C23" s="18">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="2:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="16"/>
     </row>
@@ -1043,7 +1083,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="11"/>
     </row>

</xml_diff>

<commit_message>
synthesis file done, todo => create dashboard
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_6\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BEFCF-95DA-4D85-9BFC-3AA732610E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46A7D13-8A3F-4CF7-8DB5-CC7EFB60B53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Tri plus approfondi possible</t>
   </si>
   <si>
-    <t>utilisation après coup de AmChart ou si pas de temps Voilà</t>
-  </si>
-  <si>
     <t>lowercase, retrait des mot parasite (stop_word)</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>tokenisation et lemmatization</t>
+  </si>
+  <si>
+    <t>utilisation de AmChart ou si pas de temps Voilà</t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,7 +866,7 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C8,C10:C16,C18:C20,C22:C25)</f>
-        <v>0.85000000000000009</v>
+        <v>0.98888888888888893</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="64" customHeight="1" x14ac:dyDescent="0.35">
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
@@ -961,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
@@ -983,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -994,10 +994,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="99" x14ac:dyDescent="0.35">
@@ -1023,10 +1023,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1034,10 +1034,10 @@
         <v>21</v>
       </c>
       <c r="C20" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1063,10 +1063,10 @@
         <v>24</v>
       </c>
       <c r="C23" s="18">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D24" s="16"/>
     </row>
@@ -1083,7 +1083,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D25" s="11"/>
     </row>

</xml_diff>